<commit_message>
Stopped tracking text and excel files
stopped tracking those files to avoid clashes if the code is to change
</commit_message>
<xml_diff>
--- a/multipliers.xlsx
+++ b/multipliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C280"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3402,19 +3402,682 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>4.26</t>
-        </is>
+      <c r="A229" t="n">
+        <v>4.26</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
           <t>2024-08-06 13:31:18</t>
         </is>
       </c>
-      <c r="C229" t="inlineStr">
-        <is>
-          <t>4833</t>
+      <c r="C229" t="n">
+        <v>4833</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:31:57</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>4837</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:32:19</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
+        <v>5140</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:32:40</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:32:58</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:33:27</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>3652</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:33:56</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>4729</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:34:28</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>5047</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:35:02</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>4347</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:35:22</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>4910</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:35:38</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:35:53</t>
+        </is>
+      </c>
+      <c r="C240" t="n">
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:36:12</t>
+        </is>
+      </c>
+      <c r="C241" t="n">
+        <v>3226</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:36:47</t>
+        </is>
+      </c>
+      <c r="C242" t="n">
+        <v>2874</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:37:11</t>
+        </is>
+      </c>
+      <c r="C243" t="n">
+        <v>3969</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:37:28</t>
+        </is>
+      </c>
+      <c r="C244" t="n">
+        <v>3568</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:37:46</t>
+        </is>
+      </c>
+      <c r="C245" t="n">
+        <v>2801</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:38:14</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>2590</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:38:32</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:39:00</t>
+        </is>
+      </c>
+      <c r="C248" t="n">
+        <v>2774</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:39:25</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>2992</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:39:51</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>3383</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:40:11</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>3570</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:40:31</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>2987</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:40:48</t>
+        </is>
+      </c>
+      <c r="C253" t="n">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:41:07</t>
+        </is>
+      </c>
+      <c r="C254" t="n">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:41:26</t>
+        </is>
+      </c>
+      <c r="C255" t="n">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="n">
+        <v>2.89</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:41:55</t>
+        </is>
+      </c>
+      <c r="C256" t="n">
+        <v>2251</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:42:18</t>
+        </is>
+      </c>
+      <c r="C257" t="n">
+        <v>2892</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:42:35</t>
+        </is>
+      </c>
+      <c r="C258" t="n">
+        <v>2635</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:42:52</t>
+        </is>
+      </c>
+      <c r="C259" t="n">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:43:13</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:43:44</t>
+        </is>
+      </c>
+      <c r="C261" t="n">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="n">
+        <v>6.51</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:44:20</t>
+        </is>
+      </c>
+      <c r="C262" t="n">
+        <v>2616</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:44:41</t>
+        </is>
+      </c>
+      <c r="C263" t="n">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:45:01</t>
+        </is>
+      </c>
+      <c r="C264" t="n">
+        <v>2674</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:45:29</t>
+        </is>
+      </c>
+      <c r="C265" t="n">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:45:44</t>
+        </is>
+      </c>
+      <c r="C266" t="n">
+        <v>2980</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:46:10</t>
+        </is>
+      </c>
+      <c r="C267" t="n">
+        <v>2295</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:46:31</t>
+        </is>
+      </c>
+      <c r="C268" t="n">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:46:54</t>
+        </is>
+      </c>
+      <c r="C269" t="n">
+        <v>2374</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="n">
+        <v>44.77</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:47:51</t>
+        </is>
+      </c>
+      <c r="C270" t="n">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:48:18</t>
+        </is>
+      </c>
+      <c r="C271" t="n">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:48:46</t>
+        </is>
+      </c>
+      <c r="C272" t="n">
+        <v>3059</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="n">
+        <v>26.65</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:49:38</t>
+        </is>
+      </c>
+      <c r="C273" t="n">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="n">
+        <v>2.94</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:50:07</t>
+        </is>
+      </c>
+      <c r="C274" t="n">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:50:26</t>
+        </is>
+      </c>
+      <c r="C275" t="n">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:50:49</t>
+        </is>
+      </c>
+      <c r="C276" t="n">
+        <v>3290</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:51:06</t>
+        </is>
+      </c>
+      <c r="C277" t="n">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:51:42</t>
+        </is>
+      </c>
+      <c r="C278" t="n">
+        <v>2941</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:52:10</t>
+        </is>
+      </c>
+      <c r="C279" t="n">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>1.08</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>2024-08-06 13:52:31</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>4064</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
80% done with the merged scrapper bot
pressures
- after placing the bet, the multiplier value is not scrapped
- after a successful cashout, the incremented value is not reset
</commit_message>
<xml_diff>
--- a/multipliers.xlsx
+++ b/multipliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C436"/>
+  <dimension ref="A1:C462"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6957,9 +6957,399 @@
           <t>2024-08-09 17:19:46</t>
         </is>
       </c>
-      <c r="C436" t="inlineStr">
-        <is>
-          <t>6203</t>
+      <c r="C436" t="n">
+        <v>6203</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>6.62</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>2024-08-11 20:52:17</t>
+        </is>
+      </c>
+      <c r="C437" t="n">
+        <v>5438</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>5.15</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:00:36</t>
+        </is>
+      </c>
+      <c r="C438" t="n">
+        <v>4149</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:00:53</t>
+        </is>
+      </c>
+      <c r="C439" t="n">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:01:22</t>
+        </is>
+      </c>
+      <c r="C440" t="n">
+        <v>3883</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:01:48</t>
+        </is>
+      </c>
+      <c r="C441" t="n">
+        <v>4508</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>4.93</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:05:43</t>
+        </is>
+      </c>
+      <c r="C442" t="n">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>4.93</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:06:09</t>
+        </is>
+      </c>
+      <c r="C443" t="n">
+        <v>4236</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>4.96</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:11:19</t>
+        </is>
+      </c>
+      <c r="C444" t="n">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:11:39</t>
+        </is>
+      </c>
+      <c r="C445" t="n">
+        <v>4919</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1.70</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:12:04</t>
+        </is>
+      </c>
+      <c r="C446" t="n">
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1.14</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:12:21</t>
+        </is>
+      </c>
+      <c r="C447" t="n">
+        <v>4721</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1.18</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:14:16</t>
+        </is>
+      </c>
+      <c r="C448" t="n">
+        <v>2926</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1.91</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:14:51</t>
+        </is>
+      </c>
+      <c r="C449" t="n">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1.04</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:17:50</t>
+        </is>
+      </c>
+      <c r="C450" t="n">
+        <v>2767</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1.97</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:18:35</t>
+        </is>
+      </c>
+      <c r="C451" t="n">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1.11</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:18:53</t>
+        </is>
+      </c>
+      <c r="C452" t="n">
+        <v>2910</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>347.84</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:24:34</t>
+        </is>
+      </c>
+      <c r="C453" t="n">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>2.44</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:25:05</t>
+        </is>
+      </c>
+      <c r="C454" t="n">
+        <v>4049</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1.11</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:25:25</t>
+        </is>
+      </c>
+      <c r="C455" t="n">
+        <v>4292</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1.11</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:25:26</t>
+        </is>
+      </c>
+      <c r="C456" t="n">
+        <v>4292</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1.36</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:26:24</t>
+        </is>
+      </c>
+      <c r="C457" t="n">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1.64</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:26:59</t>
+        </is>
+      </c>
+      <c r="C458" t="n">
+        <v>4589</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:27:21</t>
+        </is>
+      </c>
+      <c r="C459" t="n">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:27:57</t>
+        </is>
+      </c>
+      <c r="C460" t="n">
+        <v>3791</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>2.75</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:28:36</t>
+        </is>
+      </c>
+      <c r="C461" t="n">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1.13</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:28:53</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>4690</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented new login functionality on the scrapper
just that guy!
</commit_message>
<xml_diff>
--- a/multipliers.xlsx
+++ b/multipliers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C462"/>
+  <dimension ref="A1:C463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7347,9 +7347,24 @@
           <t>2024-08-11 21:28:53</t>
         </is>
       </c>
-      <c r="C462" t="inlineStr">
-        <is>
-          <t>4690</t>
+      <c r="C462" t="n">
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>2024-08-11 21:38:52</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>4229</t>
         </is>
       </c>
     </row>

</xml_diff>